<commit_message>
Implemented file lock via copy on .xlsx and save check before exiting.
</commit_message>
<xml_diff>
--- a/Test/singlecat.xlsx
+++ b/Test/singlecat.xlsx
@@ -29,7 +29,7 @@
     <t>D0001</t>
   </si>
   <si>
-    <t>DEMO 1 HJK WITH SOME MORE</t>
+    <t>DEMO 1 HJK WITH SOME MORE AND A CHANGE</t>
   </si>
   <si>
     <t>D0002</t>
@@ -41,7 +41,7 @@
     <t>D0003</t>
   </si>
   <si>
-    <t xml:space="preserve">REMOVE EVERYTHING. DEMO 2 ZZX ZZ. </t>
+    <t>REMOVE EVERYTHING. DEMO 2 ZZX ZZ.</t>
   </si>
   <si>
     <t>disabled</t>

</xml_diff>

<commit_message>
Added basic tests for knm with testfile2.xlsx
</commit_message>
<xml_diff>
--- a/Test/singlecat.xlsx
+++ b/Test/singlecat.xlsx
@@ -29,7 +29,7 @@
     <t>D0001</t>
   </si>
   <si>
-    <t>DEMO 1 HJK WITH SOME MORE AND A CHANGE</t>
+    <t>DEMO 1 HJK WITH SOME MORE</t>
   </si>
   <si>
     <t>D0002</t>
@@ -41,7 +41,7 @@
     <t>D0003</t>
   </si>
   <si>
-    <t>REMOVE EVERYTHING. DEMO 2 ZZX ZZ.</t>
+    <t xml:space="preserve">REMOVE EVERYTHING. DEMO 2 ZZX ZZ. </t>
   </si>
   <si>
     <t>disabled</t>

</xml_diff>

<commit_message>
Simplified keynote creation logic
</commit_message>
<xml_diff>
--- a/Test/singlecat.xlsx
+++ b/Test/singlecat.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
   <si>
     <t>General</t>
   </si>
@@ -26,58 +26,76 @@
     <t>GENERAL</t>
   </si>
   <si>
+    <t>D0000</t>
+  </si>
+  <si>
+    <t>DEMO 1 HJK WITH SOME MORE</t>
+  </si>
+  <si>
     <t>D0001</t>
   </si>
   <si>
-    <t>DEMO 1 HJK WITH SOME MORE</t>
+    <t>DEMO 2 ZZX ZZ. THIS IS GOING TO BE A LONGER LINE, WITH SEVERAL BITS OF NEW STUFF. AND ACTIVE. NO NEWLINES ALLOWED. DEMO 2 ZZX ZZ. THIS IS GOING TO BE A LONGER LINE.</t>
   </si>
   <si>
     <t>D0002</t>
   </si>
   <si>
-    <t>DEMO 2 ZZX ZZ. THIS IS GOING TO BE A LONGER LINE, WITH SEVERAL BITS OF NEW STUFF. AND ACTIVE. NO NEWLINES ALLOWED. DEMO 2 ZZX ZZ. THIS IS GOING TO BE A LONGER LINE.</t>
+    <t xml:space="preserve">REMOVE EVERYTHING. DEMO 2 ZZX ZZ. </t>
+  </si>
+  <si>
+    <t>disabled</t>
   </si>
   <si>
     <t>D0003</t>
   </si>
   <si>
-    <t xml:space="preserve">REMOVE EVERYTHING. DEMO 2 ZZX ZZ. </t>
-  </si>
-  <si>
-    <t>disabled</t>
+    <t>&lt;EMPTY&gt;</t>
   </si>
   <si>
     <t>D0004</t>
   </si>
   <si>
-    <t>&lt;EMPTY&gt;</t>
+    <t>&lt;Empty&gt;</t>
   </si>
   <si>
     <t>DO NOT USE THIS ROW, INSERT NEW ROW AS NEEDED</t>
   </si>
   <si>
+    <t>E0000</t>
+  </si>
+  <si>
+    <t>EXISTING 1 DON’T TOUCH ME!</t>
+  </si>
+  <si>
     <t>E0001</t>
   </si>
   <si>
-    <t>EXISTING 1 DON’T TOUCH ME!</t>
+    <t>EXISTING 2</t>
   </si>
   <si>
     <t>E0002</t>
   </si>
   <si>
-    <t>EXISTING 2</t>
+    <t>E0003</t>
+  </si>
+  <si>
+    <t>E0004</t>
+  </si>
+  <si>
+    <t>N0000</t>
+  </si>
+  <si>
+    <t>NEW ONE.</t>
   </si>
   <si>
     <t>N0001</t>
   </si>
   <si>
-    <t>NEW ONE.</t>
+    <t>MAKE ALL THE NEW WORK PRETTY.</t>
   </si>
   <si>
     <t>N0002</t>
-  </si>
-  <si>
-    <t>MAKE ALL THE NEW WORK PRETTY.</t>
   </si>
 </sst>
 </file>
@@ -441,7 +459,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,20 +532,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="5" t="s">
+    <row r="9" spans="1:3">
+      <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="B9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="4" t="s">
+      <c r="A11" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -537,48 +555,103 @@
       <c r="B12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="5" t="s">
-        <v>12</v>
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="6" t="s">
-        <v>17</v>
+      <c r="A15" t="s">
+        <v>20</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" t="n">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="6" t="s">
-        <v>19</v>
+      <c r="A16" t="s">
+        <v>21</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" t="n">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A11:C11"/>
     <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A23:C23"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>